<commit_message>
fixed a couple bugs and added supporting evidence folder
</commit_message>
<xml_diff>
--- a/backends/upload-app/templates/Scoping Document.xlsx
+++ b/backends/upload-app/templates/Scoping Document.xlsx
@@ -399,7 +399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
@@ -1269,6 +1269,173 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Insperity</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>This system is primarily used for HR management and payroll processing. It supports employee onboarding, I-9 verifications, benefits elections, payroll data submission, time reporting, and vacation accrual tracking.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The client utilizes this system to manage onboarding processes, employee benefit elections, vacation time tracking, payroll processing, and manual compensation adjustments within employee profiles.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>The HR team, led by Laurie Stewart (Senior Vice President of HR), oversees system administration and user access management.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>HR inputs new hire details such as salary, start date, and manager into the system, triggering onboarding notifications and granting employee access to Insperity, while elevated access or role changes require an admin-submitted access request form reviewed and provisioned by the Insperity team.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Upon termination, HR updates the employee's record with the termination date and reason. For standard employees, limited access is retained for viewing tax forms, while for elevated access users, an email is sent to Insperity to request access removal, and confirmation is documented via email.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Access is configured using a permission-based model, where specific permissions are selected through an access request form and provisioned by the Insperity team; users cannot create roles or grant access themselves.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>No; Access is permission-based, and system administrators cannot create or modify roles. Changes to permissions require submitting an access request form, which is processed and provisioned by the Insperity team.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>No; management intends to implement periodic reviews of elevated user access in the future, but no formal review process for all roles and permissions currently exists.</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Yes; Users with privileged access include the HR team, Megan Hodgson, John, Laurie Stewart, and Heather Malcolm, who have admin access to manage system configurations and employee setups, with some actions requiring external intervention.</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>No; there are no interactive system accounts within the system.</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Yes; but periodic user access reviews for elevated users are not currently being performed. Management plans to implement this process going forward.</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>No, the system does not have activity logging capabilities or audit trail functionality.</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>No; periodic activity reviews of user activity are not currently performed, but there are indirect controls in place such as payroll reviews.</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Users authenticate through direct login with enforced two-factor authentication for all accounts.</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>No; The client does not perform periodic reviews of the system's authentication configurations.</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Management does not have the ability to make any changes to this system. All system configurations, workflows, and code are managed entirely by the vendor.</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Access to make changes is restricted to Megan Hodgson, John, and the HR team. Megan and John have administrative access due to the current size of the team and operational needs, while the HR team has admin access to manage application configurations.</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Management does not have any separate environments for this system.</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>The client's change management process includes the following steps: Access provisioning changes are requested via an access request form specifying permissions, approved by Insperity, and deployed by Insperity support without client-side provisioning. Payroll changes are requested via email, reviewed and approved by Megan and John, and implemented by Insperity after client approval. User access termination requests are sent via email, confirmed by Insperity, and access is disabled. Payroll data is reviewed semi-monthly by Megan and John, who approve and finalize it for submission. Changes are logged in a pay change history report, and future plans include implementing a new payroll system with formalized controls.</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>No, the vendor manages all updates, patches, and bug fixes directly in the production environment. The client has no ability to make changes or updates themselves, and there is no sandbox or QA environment for testing.</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>The system enforces segregation of duties through inherent controls. Users cannot independently provision access, make configuration changes, or modify payroll data, as these actions are handled by Insperity support. Additionally, the system includes audit logging and two-factor authentication to enhance security and monitoring.</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>No periodic review of changes is performed.</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Yes, the system has automated jobs or interfaces with benefits administration sites and their website. These jobs perform functions related to benefits management and payroll journal entry preparation.</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>Jobs are managed using vendor-managed tools provided by Insperity. These tools handle scheduling and monitoring of automated processes, while the organization does not currently use internal systems for these functions.</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>Data is stored in a vendor-managed database managed by Insperity.</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>Backups are handled entirely by the vendor as part of their SaaS service.</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>No, management does not perform regular SOC report reviews.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Couple of bug fixes
</commit_message>
<xml_diff>
--- a/backends/upload-app/templates/Scoping Document.xlsx
+++ b/backends/upload-app/templates/Scoping Document.xlsx
@@ -399,7 +399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG6"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
@@ -1436,6 +1436,173 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Insperity</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>This system is primarily used for HR management and employee administration. It supports onboarding, I-9 verification, benefits election, payroll processing, time reporting, vacation accruals, and time tracking.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>The client utilizes this system to manage onboarding processes, employee benefit elections, time tracking for vacation accruals, payroll processing, and manual compensation updates within employee profiles.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>The HR team, led by Laurie Stewart (SVP of HR), manages system administration and user access.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Access provisioning is initiated when HR inputs details such as salary, start date, and manager information for new hires, triggering a notification for onboarding paperwork and granting employee access to Insperity. Elevated access requires an admin to submit a permission-based access request form to the Insperity team for provisioning, as Jade users cannot directly provision access. Role changes are not explicitly detailed but likely follow the elevated access request process.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Upon termination, HR updates the employee's termination date and reason in the system. For elevated access users, an email is sent to Insperity to request access removal, and confirmation is received via email documenting the process.</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Access is configured using a permission-based model, where specific permissions are selected through an access request form and provisioned by the Insperity team.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>No; Access is permission-based, and system administrators cannot create, modify, or delete roles. Changes to permissions require submission of an access request form processed by the vendor.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Yes; Users with privileged access include Megan Hodgson, John, and the HR team, who can perform unrestricted functions such as setting up new employees, though payroll processing is controlled externally by Insperity.</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>No; there are no interactive system accounts within the system.</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>The credentials for all accounts are fully managed and stored by Insperity's system; there is no local storage or management of these credentials by the Jade team.</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>N/A - No Interactive System Accounts</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Yes; Management will perform periodic user access reviews. No additional detail was provided regarding the frequency or process during the walkthrough meeting.</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>The system maintains logs of pay change activities. Logs include change history details but do not explicitly confirm comprehensive admin activity logging or audit trail functionality.</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>No; periodic activity reviews of user activity are not currently performed, but there are related controls such as payroll reviews and plans to implement user access reviews in the future.</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Users authenticate through direct login with enforced two-factor authentication for all accounts.</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>No; The client does not perform periodic reviews of the systems authentication configurations.</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Management does not have the ability to make any changes to this system. All system configurations, workflows, and code are managed entirely by the vendor.</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Access to make changes is restricted to Megan Hodgson, John, and the HR team, who have administrative access to the application. Megan and John have admin access due to the current size of the team and operational needs, while the HR team has admin access for managing system configurations. All change access is granted through role-based permissions in the system.</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Management does not have any separate environments for this system.</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>The change management process varies by change type. Access changes require an access request form specifying permissions, internal approval, and provisioning by Insperity, with Jade employees restricted from direct modifications. Payroll changes are requested via email, reviewed internally by designated personnel, and processed by Insperity with draft reviews for approval. Termination of user access involves email requests to Insperity, documented approvals, and confirmation of access disablement. Periodic payroll reviews serve as indirect validation of payroll changes, and a pay change history report tracks payroll-related modifications. There is no formalized process for testing and development, but plans to implement a new payroll system suggest future formalization of change management controls.</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>No, the vendor manages all updates, patches, and bug fixes directly in the production environment. The client does not have a sandbox or QA environment, and no changes are made internally by the client's IT team.</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>No periodic review of changes is performed.</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>No automated jobs or interfaces are currently implemented for this system.</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>The tools used to run, schedule, and monitor the automated jobs were not identified, and no specific capabilities were discussed.</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>The failure resolution process involves contacting Insperity's support team, waiting for them to resolve the issue, and relying on vendor-managed operations for backups and system-related issues.</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>Data is stored in vendor-managed systems handled by Insperity.</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>Backups are handled entirely by the vendor as part of their SaaS service.</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>N/A - All backup types and strategies are managed by the vendor as part of their SaaS service.</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>N/A - the vendor is responsible for monitoring and resolving any backup failures.</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>No, management does not perform regular SOC report reviews.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
minor changes to the layout
</commit_message>
<xml_diff>
--- a/backends/upload-app/templates/Scoping Document.xlsx
+++ b/backends/upload-app/templates/Scoping Document.xlsx
@@ -399,7 +399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG1"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
@@ -601,7 +601,173 @@
         </is>
       </c>
     </row>
-    <row r="2" customFormat="1" s="1"/>
+    <row r="2" customFormat="1" s="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>NetSuite</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>This system is primarily used for financial management, accounting, and reporting. It supports journal entries, trial balances, financial reporting, purchase order creation, and workflows for approvals.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>The client utilizes this system to manage accounting processes, purchase order workflows, bill approvals, financial reporting, and integration with payment and budgeting tools.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>The NetSuite system administration is managed by Blackforge Consulting, led by Steve Monti and Andrew Baker.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Access provisioning is initiated by an email sent by Megan Hodgson or another authorized individual, creating a ticket in Blackforge's system. The ticket requires approval from Megan Hodgson or John, with neither approving their own changes, before Blackforge executes the requested updates to roles or permissions and documents the changes in the system.</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Upon termination, access is removed immediately. NetSuite access, integrated with Azure for Single Sign-On, is manually revoked, and a screenshot of the removal is documented and shared with HR via email.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Access is configured using a role-based model, where custom roles are defined and permissions are aligned with specific functions. Global permissions are disabled, and roles were tested during user acceptance testing as part of the system rollout.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Yes; System administrators can modify roles in NetSuite, including making changes to existing roles and testing these modifications as part of the user acceptance testing process.</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Yes; management performs an annual review of all roles and permissions.</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Yes; Users with privileged access include Steve Monti, Andrew Baker, and Justin, who hold the Administrator role and can make system changes.</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Yes; there are system roles tied to individual user accounts, but no fully non-human accounts exist currently.</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Credentials for shared and integration accounts are linked to individual user accounts and are not currently stored in a formal enterprise credential management solution.</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Yes; Management performs periodic access reviews. Reviews were conducted during the initial implementation and go-live phase, with the intention to perform them quarterly moving forward.</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>The system maintains logs of administrative activities. Logs are retained indefinitely and include high-level user actions.</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>The system uses Azure SSO for authentication in the production environment, while the sandbox environment relies on independent login functionality.</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>No; The client does not perform periodic reviews of the system's authentication configurations.</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Management can perform configuration changes to adjust system settings, update workflows, modify integrations, and make limited code/script changes within the NetSuite system. These changes are managed through a ticketing system, with Blackforge handling development and deployment, and Jade's team performing testing and approvals where applicable.</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Access to make changes is restricted to a small group of administrators. Steve Monti and Andrew Baker from Blackforge Consulting have full administrator access to NetSuite as primary administrators, while Justin from Whipfli currently has administrator access for managing integration setup. All change access is granted through role-based permissions in the system.</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Management maintains separate Sandbox and Release Preview environments for implementing and testing changes.</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>The change management process varies by change type. Workflow, configuration, and script changes begin with ticket creation in Blackforge's system, followed by development in the sandbox environment, testing by Jade's team, approval by Jade's team, and deployment to production by Blackforge. Integration changes involve email requests to the integration owner, development by the owner or through NetSuite adjustments, testing in the live environment, informal approval via email, and direct deployment. Bundle audit trail changes and patches are managed by NetSuite, with Blackforge handling testing, approval, and deployment as needed. All changes follow distinct processes based on their type and risk level.</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Yes, the vendor pushes updates, patches, and bug fixes. Semiannual system upgrades are tested in a release preview environment before deployment to Production, with evidence of testing documented. Patches and bug fixes are assessed for relevance and handled on a case-by-case basis.</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>No, there is no inherent system functionality preventing users from both developing and deploying changes.</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Yes, the system has automated jobs and interfaces with Bill.com, Concur, and Adaptive Planning. These jobs perform data integration and transfer functions between systems.</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>The following tools are used: NetSuite and Adaptive. Each tool is responsible for managing integration jobs and monitoring failures, with notifications sent for task success or failure.</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Job failures are handled through a defined process: detection occurs via Adaptive's run log, notifications are sent for successful or failed runs, and resolution involves identifying the issue, creating missing mappings, and manually re-running the job.</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>The system utilizes NetSuite for data storage, which is vendor managed.</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>N/A - All backup types and strategies are managed by the vendor as part of their SaaS service.</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>N/A - Backup failure resolution is managed by the vendor as part of their SaaS service.</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>No, management does not perform regular SOC report reviews.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refining the Gap Examples
</commit_message>
<xml_diff>
--- a/backends/upload-app/templates/Scoping Document.xlsx
+++ b/backends/upload-app/templates/Scoping Document.xlsx
@@ -399,7 +399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
@@ -768,6 +768,173 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Microsoft Azure</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>This is a cloud-based platform primarily used for SSL authentication and access management. It supports user licensing, email services, collaboration tools, and document management functionalities.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>The client utilizes this system for SSL authentication and access management across different systems and for core Microsoft 365 services, including user licensing, collaboration through SharePoint, email via Exchange, and communication using Teams.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>The system is currently administered by Ralph Vaccaro, with oversight expected to transition to Nicole Tai (Vice President) upon her joining.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Access provisioning is initiated by HR sending a message with the new hire's details, including name, department, position, and start date, to the IT team, who manually create accounts prior to the start date. Elevated access requests require submission by the hiring manager or area lead and approval from IT leadership or another department head before access is granted.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Access is removed upon termination or role change when HR or the hiring manager sends an email specifying the change and effective date. The IT team deactivates access starting with Azure, which cascades to SSO-integrated systems, while non-SSO systems are handled independently.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Access is configured using a role-based model, where predefined roles such as regular user and elevated access (admin) are used, with elevated access granting full administrative privileges; currently, only one individual and a dormant backup account hold elevated access.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>No; Only vendor-provided roles exist, and the client cannot alter role definitions without vendor assistance.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>No; management does not perform periodic reviews of roles and permissions.</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Yes; Users with privileged access include Ralph Vaccaro with active admin access and a dormant IT Admin account used as a backup.</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Yes; There is an interactive IT Admin account used as a backup, and additional generic accounts exist for specific functionalities, but they do not have elevated access.</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>The credentials for the non-human IT admin account are memorized by Ralph Vaccaro, with no formal documentation or storage method.</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>The password for the IT Admin account is known only to Ralph Vaccaro and stored in his memory, while other non-human accounts with standard access are configured as regular users without elevated access.</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>No; Management does not currently perform periodic access reviews. Elevated access in Azure has not been reviewed as of today.</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>No, the system does not have activity logging capabilities or audit trail functionality.</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>No; periodic reviews of user activity, roles, permissions, or elevated access are not currently performed, and activity logging or tracking functionality is not actively utilized.</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>The system uses Azure SSO with MFA for all users, and privileged accounts include a backup non-human IT Admin account for emergency access.</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>No; The client does not perform periodic reviews of the systems authentication configurations.</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Management can modify permissions on certain restricted areas within Azure. No other types of changes, such as configuration, workflow, or code changes, are performed by management.</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Access to make changes is restricted to Ralph Vaccaro, who holds an admin role with elevated access, and the IT Admin Account, a dormant non-human account used as a backup. Ralph is the only individual with knowledge of the IT Admin Account password, ensuring controlled access to modify the system.</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Management does not have any separate environments for this system.</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>There is no formal change management process in place. Changes are requested verbally or via email, and the IT team makes changes directly in the production environment without formal approvals or testing. There is no documentation of changes, and no review process exists to validate changes were appropriate.</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>No, the vendor manages updates, patches, and bug fixes for the SaaS system. The organization does not perform independent testing or validation of these updates and relies entirely on the vendor for deployment and oversight.</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>No periodic review of changes is performed.</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>No automated jobs or interfaces are currently implemented for this system.</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>The automated jobs are configured using native system functionality and are not scheduled to run, as there are no automated jobs or interfaces currently in use between Azure and other systems.</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>The system utilizes Microsoft Azure for data storage, which is vendor-managed.</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>Backups are not currently performed independently, but implementation of Druva for 365 backups is in progress.</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>N/A - All backup types and strategies are managed by the vendor as part of their SaaS service.</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>N/A - the vendor is responsible for monitoring and resolving any backup failures.</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>No, management does not perform regular SOC report reviews.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed RCM builder so it's easier to generate gaps
</commit_message>
<xml_diff>
--- a/backends/upload-app/templates/Scoping Document.xlsx
+++ b/backends/upload-app/templates/Scoping Document.xlsx
@@ -399,7 +399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
@@ -604,62 +604,62 @@
     <row r="2" customFormat="1" s="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NetSuite</t>
+          <t>Salesforce</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>This system is primarily used for financial management, accounting, and reporting. It supports deal entries, purchase order creation, workflow management for approvals, bill approvals, payment integration, journal entries, and financial reporting.</t>
+          <t>This is a cloud-based CRM platform providing sales, marketing, and service functionalities. It supports lead management, sales tracking, and integration with financial systems for data transfer.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The client utilizes this system to manage financial processes such as journal entries, purchase orders, bill approvals, and financial reporting, while also supporting integrations with other platforms and role-based access controls.</t>
+          <t>The client utilizes this system as the primary CRM solution, tracking clients, managing sales opportunities, and transferring sales data to the ERP system.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>The NetSuite system administration is managed by Blackforge Consulting, with Steve Monti and Andrew Baker serving as primary administrators.</t>
+          <t>The Salesforce Administration Team, led by Vincent Washburn (Senior Salesforce Engineer).</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Access provisioning is initiated when Jade employees send an email to Blackforge's support email, which auto-generates a ticket in Blackforge's system. The request is reviewed and approved by authorized approvers, Megan Hodgson or John, with cross-approval for each other's changes. Blackforge executes the approved changes and documents them in their ticketing system.</t>
+          <t>Access provisioning is triggered by HR updates in Workday for new hires, which automatically create a ticket in ServiceNow. The ticket includes necessary role information and requires manager confirmation before access is provisioned by the IT team. Additional access requests are handled informally through direct communication with the IT team, bypassing a formal ticketing process. Role changes were not explicitly addressed.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Upon termination, access is removed immediately, with NetSuite access in the production environment tied to Azure SSO and sandbox access removed separately; documentation includes a screenshot of the removal sent via email and recorded in a case shared with HR.</t>
+          <t>When HR enters a termination date in Workday, an automated process creates a ServiceNow ticket, notifying system owners to remove access within three business days and requiring confirmation from the system owner before the ticket is closed.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Access is configured using a role-based model, where custom roles with specific permissions are utilized, and global permissions are disabled in the system.</t>
+          <t>Access is configured using a role-based model, where roles and permissions are determined by job titles in Workday and provisioned automatically through ServiceNow, with additional access manually granted by administrators upon informal requests.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Yes; system administrators can modify roles in NetSuite, including making changes and performing testing as part of the user acceptance testing process.</t>
+          <t>Yes; system administrators can modify roles, configurations, and integrations, and they also have access to the back-end code.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Yes; management performs an annual review of all roles and permissions.</t>
+          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Yes; Users with privileged access include Steve Monti, Andrew Baker, and Justin, who hold administrator roles and can modify system configurations and key settings.</t>
+          <t>Yes; Users with privileged access include Vincent Washburn and Jeremy, who have administrative access to the Salesforce application.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Yes; there are interactive system accounts used for integration purposes, including one for Concur and another currently linked to an individual user for Adaptive Planning.</t>
+          <t>No; there are no interactive system accounts within the system.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+          <t>N/A - No Interactive System Accounts</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -669,52 +669,52 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Yes; Reviews are conducted quarterly. Management performed an initial review during system implementation and confirmed that periodic reviews will continue on a quarterly basis moving forward.</t>
+          <t>Yes; Management conducts quarterly access reviews. Compliance initiates the process, and user access is reviewed for appropriateness during each cycle.</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Activity logging captures administrative user actions and includes logging and reporting functionality. Logs are stored within the system for an unspecified duration.</t>
+          <t>The system maintains logs of user activities. Logs are retained within Salesforce and include administrative user actions.</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+          <t>No; the system logs are not reviewed unless there is an incident</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>The system uses a hybrid authentication approach where regular users authenticate through Azure SSO for the production environment, while the sandbox environment requires independent login credentials, and privileged access is restricted to specific administrators.</t>
+          <t>The system uses a hybrid authentication approach where regular users authenticate through Okta SSO, while administrators maintain direct application credentials as a backup authentication path.</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>No; The client does not perform periodic reviews of the system's authentication configurations.</t>
+          <t>Yes; The client periodically reviews authentication configurations to ensure alignment with security standards.</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Management can perform configuration changes to adjust system settings, update workflows, modify custom scripts, and manage saved searches. These changes are handled by Blackforge through a ticketing system, with development in a sandbox environment, testing by Jade's team, and deployment to production.</t>
+          <t>Management can perform configuration changes to adjust system settings, update workflows, and modify custom code within Salesforce. These changes are managed by Vincent Washburn and his colleague Jeremy, who have the ability to develop and deploy updates in a sandbox environment before moving to production.</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Access to make changes is restricted to a small group of administrators. Steve Monti and Andrew Baker from Blackforge Consulting have elevated access to make system changes, while Justin from Whipflee has administrator access for integration setup and related changes. All change access is granted through role-based permissions in the system.</t>
+          <t>The following roles have change capabilities: Senior Salesforce Engineer (administrative and configuration changes) and Salesforce Engineer (administrative and configuration changes). These roles are assigned to Vincent Washburn and his colleague Jeremy, who are the only individuals with administrative access to Salesforce and are authorized to make changes to the application.</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>Management maintains separate Sandbox and Release Preview environments for implementing and testing changes.</t>
+          <t>Management maintains a separate sandbox environment for implementing and testing changes.</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>The client's change management process varies by change type. Workflow, configuration, and script changes begin with ticket creation in Blackforge's system, followed by development and testing in the sandbox environment. Jade's team performs testing and provides approval before Blackforge deploys changes to production. Integration changes are requested by contacting the integration owner, with changes developed and tested directly in the live environment, followed by email approval. NetSuite quarterly release changes involve Blackforge testing in a release preview environment, with deployment managed by NetSuite. All changes maintain segregation of duties, with distinct roles for development, testing, and deployment.</t>
+          <t>The client's change management process includes the following steps: 1) Change request submission via JIRA ticket created by Vincent or Jeremy, 2) Development in the sandbox environment by Vincent or Jeremy, 3) Testing in the sandbox environment coordinated by Jeremy with relevant stakeholders, 4) Approval captured within the JIRA ticket by the Change Advisory Board (CAB) before deployment, 5) Deployment to production performed by Vincent or Jeremy without strict segregation of duties between development and deployment.</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Yes, the vendor pushes updates, patches, and bug fixes on a case-by-case basis when issues are identified or complaints are received. Notifications from the vendor are reviewed by Blackforge Consulting, but there is no formalized process for testing or validating these updates before deployment.</t>
+          <t>Yes, the vendor manages updates, patches, and bug fixes for the SaaS system, but the specific process for deploying these changes to production was not discussed.</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -724,22 +724,22 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>Management performs periodic reviews of system changes to ensure they were appropriately requested, tested, and approved prior to deployment. The review process includes validating documentation in the ticketing system, such as change requests, test results, approvals, and deployment records, with any discrepancies addressed by Jade's team and Blackforge.</t>
+          <t>No periodic review of changes is performed.</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Yes, the system has three types of automated jobs/interfaces with Bill.com, Concur, and Adaptive Planning. These jobs perform payment processing, expense management integration, and data synchronization.</t>
+          <t>Yes, the system has automated jobs and interfaces with NetSuite. These jobs transfer sales information for closed sales, including numbers and client data, using a tool that pulls data daily and transforms it for compatibility.</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>The following tools are used: NetSuite and Adaptive. Each tool is responsible for managing saved searches and exporting data as CSV files, documenting failures, and providing notifications for task statuses.</t>
+          <t>Jobs are managed using Salesforce's native functionality, NetSuite's native functionality, and Workato. These tools provide scheduling and monitoring capabilities for automated jobs and interfaces.</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>Job failures are handled through a defined process: 1) failures are documented in Adaptive, 2) notifications are sent for both successful and failed tasks, 3) resolution involves creating missing accounts in Adaptive, remapping, and rerunning the task.</t>
+          <t>Job failures are handled through a defined process: detection is performed manually by the accounting team, notification occurs when the accounting team informs the IT team of issues, resolution involves reviewing Workato logs and rerunning the job or opening a ticket for complex problems.</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
@@ -754,184 +754,17 @@
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+          <t>N/A - All backup types and strategies are managed by the vendor as part of their SaaS service.</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>N/A - Backup failure resolution is managed by the vendor as part of their SaaS service.</t>
+          <t>Backup failures are addressed through monitoring by the accounting team, notification to the IT team, review of Workato logs to identify errors, rerunning the job to resolve issues, and opening a ticket for complex problems with resolution logged in the ticket.</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Microsoft Azure</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>This is a cloud-based platform primarily used for SSL authentication and access management. It supports user licensing, email services, collaboration tools, and document management functionalities.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>The client utilizes this system for SSL authentication and access management across different systems and for core Microsoft 365 services, including user licensing, collaboration through SharePoint, email via Exchange, and communication using Teams.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>The system is currently administered by Ralph Vaccaro, with oversight expected to transition to Nicole Tai (Vice President) upon her joining.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Access provisioning is initiated by HR sending a message with the new hire's details, including name, department, position, and start date, to the IT team, who manually create accounts prior to the start date. Elevated access requests require submission by the hiring manager or area lead and approval from IT leadership or another department head before access is granted.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Access is removed upon termination or role change when HR or the hiring manager sends an email specifying the change and effective date. The IT team deactivates access starting with Azure, which cascades to SSO-integrated systems, while non-SSO systems are handled independently.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Access is configured using a role-based model, where predefined roles such as regular user and elevated access (admin) are used, with elevated access granting full administrative privileges; currently, only one individual and a dormant backup account hold elevated access.</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>No; Only vendor-provided roles exist, and the client cannot alter role definitions without vendor assistance.</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>No; management does not perform periodic reviews of roles and permissions.</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Yes; Users with privileged access include Ralph Vaccaro with active admin access and a dormant IT Admin account used as a backup.</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Yes; There is an interactive IT Admin account used as a backup, and additional generic accounts exist for specific functionalities, but they do not have elevated access.</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>The credentials for the non-human IT admin account are memorized by Ralph Vaccaro, with no formal documentation or storage method.</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>The password for the IT Admin account is known only to Ralph Vaccaro and stored in his memory, while other non-human accounts with standard access are configured as regular users without elevated access.</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>No; Management does not currently perform periodic access reviews. Elevated access in Azure has not been reviewed as of today.</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>No, the system does not have activity logging capabilities or audit trail functionality.</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>No; periodic reviews of user activity, roles, permissions, or elevated access are not currently performed, and activity logging or tracking functionality is not actively utilized.</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>The system uses Azure SSO with MFA for all users, and privileged accounts include a backup non-human IT Admin account for emergency access.</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>No; The client does not perform periodic reviews of the systems authentication configurations.</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Management can modify permissions on certain restricted areas within Azure. No other types of changes, such as configuration, workflow, or code changes, are performed by management.</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Access to make changes is restricted to Ralph Vaccaro, who holds an admin role with elevated access, and the IT Admin Account, a dormant non-human account used as a backup. Ralph is the only individual with knowledge of the IT Admin Account password, ensuring controlled access to modify the system.</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Management does not have any separate environments for this system.</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>There is no formal change management process in place. Changes are requested verbally or via email, and the IT team makes changes directly in the production environment without formal approvals or testing. There is no documentation of changes, and no review process exists to validate changes were appropriate.</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>No, the vendor manages updates, patches, and bug fixes for the SaaS system. The organization does not perform independent testing or validation of these updates and relies entirely on the vendor for deployment and oversight.</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>No periodic review of changes is performed.</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>No automated jobs or interfaces are currently implemented for this system.</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>The automated jobs are configured using native system functionality and are not scheduled to run, as there are no automated jobs or interfaces currently in use between Azure and other systems.</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>The system utilizes Microsoft Azure for data storage, which is vendor-managed.</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>Backups are not currently performed independently, but implementation of Druva for 365 backups is in progress.</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>N/A - All backup types and strategies are managed by the vendor as part of their SaaS service.</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>N/A - the vendor is responsible for monitoring and resolving any backup failures.</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>No, management does not perform regular SOC report reviews.</t>
+          <t>Yes, management performs annual SOC 1 Type 2 report reviews. The review process includes evaluating complementary user entity controls and subservice providers and is documented in the compliance team's review template.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
couple of updates to instructions
</commit_message>
<xml_diff>
--- a/backends/upload-app/templates/Scoping Document.xlsx
+++ b/backends/upload-app/templates/Scoping Document.xlsx
@@ -609,12 +609,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>This is a cloud-based CRM platform providing sales, marketing, and service functionalities. It supports lead management, sales tracking, and integration with financial systems for data transfer.</t>
+          <t>This is a cloud-based CRM platform providing sales, marketing, and lead management functionalities. It supports client tracking, sales updates, and integration with financial systems.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The client utilizes this system as the primary CRM solution, tracking clients, managing sales opportunities, and transferring sales data to the ERP system.</t>
+          <t>The client utilizes this system as the primary CRM solution, tracking clients, managing sales opportunities, and integrating sales data with the ERP system for streamlined processing.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -624,52 +624,52 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Access provisioning is triggered by HR updates in Workday for new hires, which automatically create a ticket in ServiceNow. The ticket includes necessary role information and requires manager confirmation before access is provisioned by the IT team. Additional access requests are handled informally through direct communication with the IT team, bypassing a formal ticketing process. Role changes were not explicitly addressed.</t>
+          <t>Access provisioning is triggered by HR updates in Workday, which automatically create a ticket in ServiceNow containing necessary role information. The ticket is reviewed by the manager for access verification, and if aligned with the job title, the IT admin provisions access.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>When HR enters a termination date in Workday, an automated process creates a ServiceNow ticket, notifying system owners to remove access within three business days and requiring confirmation from the system owner before the ticket is closed.</t>
+          <t>When HR enters a termination date in Workday, an automated process creates a ServiceNow ticket, notifying system owners to remove access within three business days. Access removal is confirmed by the system owner before the ticket is closed.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Access is configured using a role-based model, where roles and permissions are determined by job titles in Workday and provisioned automatically through ServiceNow, with additional access manually granted by administrators upon informal requests.</t>
+          <t>Access is configured using a role-based model, where permissions are provisioned based on job titles recorded in Workday, and additional access can be manually granted by administrators upon request.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Yes; system administrators can modify roles, configurations, and integrations, and they also have access to the back-end code.</t>
+          <t>Yes; system administrators can modify roles in Salesforce, including configuration and workflow changes.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>N/A - This information was not discussed in the walkthrough meeting transcript.</t>
+          <t>No; management only looks at roles/permissions when an issue arises or new roles are created.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Yes; Users with privileged access include Vincent Washburn and Jeremy, who have administrative access to the Salesforce application.</t>
+          <t>Yes; Users with privileged access include Vincent Washburn, a Senior Salesforce Engineer, and Jeremy, a Salesforce Engineer, who can make changes, provision access, and perform administrative tasks.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>No; there are no interactive system accounts within the system.</t>
+          <t>Yes; there are system accounts within Salesforce used for integrations, but they are non-interactive and no team members have access to their credentials.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>N/A - No Interactive System Accounts</t>
+          <t>The credentials for the integration account are not stored in a traditional manner; token-based authentication is used, and no one has access to the credentials once set up.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>N/A - No Interactive System Accounts</t>
+          <t>No one has access to the credentials for shared or generic accounts as these accounts use token-based authentication and do not require manual credential management.</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Yes; Management conducts quarterly access reviews. Compliance initiates the process, and user access is reviewed for appropriateness during each cycle.</t>
+          <t>Yes; Management conducts quarterly access reviews. The compliance team initiates the process, and user access is reviewed for appropriateness on a quarterly basis.</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -694,27 +694,27 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Management can perform configuration changes to adjust system settings, update workflows, and modify custom code within Salesforce. These changes are managed by Vincent Washburn and his colleague Jeremy, who have the ability to develop and deploy updates in a sandbox environment before moving to production.</t>
+          <t>Management can perform configuration changes to adjust system settings, update workflows, and modify custom code within Salesforce. These changes can include adding or removing integrations, configuring discount codes, setting up approval workflows, and making updates to Apex code.</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>The following roles have change capabilities: Senior Salesforce Engineer (administrative and configuration changes) and Salesforce Engineer (administrative and configuration changes). These roles are assigned to Vincent Washburn and his colleague Jeremy, who are the only individuals with administrative access to Salesforce and are authorized to make changes to the application.</t>
+          <t>The following roles have change capabilities: Senior Salesforce Engineer (configuration, integration, workflow, and backend code changes) and Salesforce Engineer (configuration, integration, workflow, and backend code changes). These roles are assigned to Vincent Washburn and Jeremy, who are the only individuals with administrative access to Salesforce and authorized to make changes to the application.</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>Management maintains a separate sandbox environment for implementing and testing changes.</t>
+          <t>Management maintains a separate sandbox environment for implementing and testing changes prior to deployment.</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>The client's change management process includes the following steps: 1) Change request submission via JIRA ticket created by Vincent or Jeremy, 2) Development in the sandbox environment by Vincent or Jeremy, 3) Testing in the sandbox environment coordinated by Jeremy with relevant stakeholders, 4) Approval captured within the JIRA ticket by the Change Advisory Board (CAB) before deployment, 5) Deployment to production performed by Vincent or Jeremy without strict segregation of duties between development and deployment.</t>
+          <t>The client's change management process includes the following steps: Change requests are initiated verbally or via informal communication and logged in Jira, where the Change Advisory Board (CAB) is tagged for approval before development begins. Configuration and code changes are developed in the sandbox environment by Vincent or Jeremy, with testing coordinated directly with stakeholders to validate functionality. Approval is documented within the Jira ticket by the CAB, and deployment to production is performed by Vincent or Jeremy without strict segregation of duties. There is no formal process for periodic reviews of changes or enforcement of segregation between development and deployment activities.</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Yes, the vendor manages updates, patches, and bug fixes for the SaaS system, but the specific process for deploying these changes to production was not discussed.</t>
+          <t>Yes, the vendor manages updates, patches, and bug fixes for the SaaS system, but the specific process for deploying these changes to Production was not discussed.</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -729,17 +729,17 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Yes, the system has automated jobs and interfaces with NetSuite. These jobs transfer sales information for closed sales, including numbers and client data, using a tool that pulls data daily and transforms it for compatibility.</t>
+          <t>Yes, the system has automated jobs and interfaces with NetSuite. These jobs transfer sales information for closed sales from Salesforce to NetSuite daily.</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>Jobs are managed using Salesforce's native functionality, NetSuite's native functionality, and Workato. These tools provide scheduling and monitoring capabilities for automated jobs and interfaces.</t>
+          <t>The following tools are used: Salesforce native functionality and Workato. Each tool is responsible for staging integration tables and pulling, transforming, and scheduling data for processing.</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>Job failures are handled through a defined process: detection is performed manually by the accounting team, notification occurs when the accounting team informs the IT team of issues, resolution involves reviewing Workato logs and rerunning the job or opening a ticket for complex problems.</t>
+          <t>Job failures are handled through a defined process: 1) detection is performed manually by the accounting team, 2) the accounting team notifies the IT team upon identifying an issue, 3) the IT team reviews logs and typically resolves the issue by rerunning the job or opening a ticket for complex cases.</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>Backup failures are addressed through monitoring by the accounting team, notification to the IT team, review of Workato logs to identify errors, rerunning the job to resolve issues, and opening a ticket for complex problems with resolution logged in the ticket.</t>
+          <t>N/A - the vendor is responsible for monitoring and resolving any backup failures.</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">

</xml_diff>